<commit_message>
Update and delete files
</commit_message>
<xml_diff>
--- a/Time schedule (1).xlsx
+++ b/Time schedule (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.giannakakos\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Documents\VU vakken\OBP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFED140-DC01-42F3-90AA-73568C1520EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58D7358-6AE1-4EE1-9D67-39E28CCA7035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeTracking" sheetId="3" r:id="rId1"/>
@@ -18,13 +18,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>NAME</t>
   </si>
@@ -87,13 +87,19 @@
   </si>
   <si>
     <t>Time Tracking Table</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Wrote the functions to get  the information to make the class eldery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -128,6 +134,20 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -189,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -202,9 +222,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -220,12 +237,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
         <right style="thin">
           <color indexed="64"/>
@@ -362,14 +393,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="6" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
     </dxf>
@@ -389,7 +412,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Giannakakos Panagiotis" refreshedDate="45301.604413078705" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="10" xr:uid="{1BB8C3BC-4C44-4166-98EF-5CD7637D7CB0}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:E11" sheet="DATA"/>
+    <worksheetSource ref="A1:F11" sheet="DATA"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="NAME" numFmtId="0">
@@ -503,7 +526,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FA8CAA57-1BC3-44FF-B561-35A49C0A42E4}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FA8CAA57-1BC3-44FF-B561-35A49C0A42E4}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -576,63 +599,72 @@
     <dataField name="Sum of HOURS" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="22">
-    <format dxfId="21">
+    <format dxfId="22">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
+    <format dxfId="20">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
     <format dxfId="19">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
     <format dxfId="18">
-      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
     <format dxfId="17">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
     <format dxfId="16">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
+    <format dxfId="15">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
     <format dxfId="14">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
     <format dxfId="13">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
     <format dxfId="12">
-      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
     <format dxfId="11">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
     <format dxfId="10">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
+    <format dxfId="9">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
     <format dxfId="8">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+      <pivotArea field="0" dataOnly="0" grandRow="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
     </format>
     <format dxfId="7">
       <pivotArea field="0" dataOnly="0" grandRow="1" axis="axisRow" fieldPosition="0">
@@ -644,22 +676,13 @@
       </pivotArea>
     </format>
     <format dxfId="6">
-      <pivotArea field="0" dataOnly="0" grandRow="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -669,7 +692,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="4">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -679,7 +702,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -689,7 +712,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -699,7 +722,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="1">
       <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
@@ -920,38 +943,38 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -963,7 +986,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -983,87 +1006,87 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="10">
-        <v>2</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10">
-        <v>2</v>
-      </c>
-      <c r="F5" s="10">
+      <c r="B5" s="9">
+        <v>2</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9">
+        <v>2</v>
+      </c>
+      <c r="F5" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10">
-        <v>2</v>
-      </c>
-      <c r="E6" s="10">
-        <v>2</v>
-      </c>
-      <c r="F6" s="10">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9">
+        <v>2</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2</v>
+      </c>
+      <c r="F6" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10">
-        <v>2</v>
-      </c>
-      <c r="E7" s="10">
-        <v>2</v>
-      </c>
-      <c r="F7" s="10">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9">
+        <v>2</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2</v>
+      </c>
+      <c r="F7" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10">
-        <v>2</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10">
-        <v>2</v>
-      </c>
-      <c r="F8" s="10">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9">
+        <v>2</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
+        <v>2</v>
+      </c>
+      <c r="F8" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10">
-        <v>2</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10">
-        <v>2</v>
-      </c>
-      <c r="F9" s="10">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
@@ -1096,197 +1119,232 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="73.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="14">
+        <v>45301</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3">
-        <v>45301</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="3">
+        <v>45301</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="14">
+        <v>45301</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3">
-        <v>45301</v>
-      </c>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="3">
+        <v>45301</v>
+      </c>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="14">
+        <v>45301</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3">
-        <v>45301</v>
-      </c>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3">
+        <v>45301</v>
+      </c>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="14">
+        <v>45301</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3">
-        <v>45301</v>
-      </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="3">
+        <v>45301</v>
+      </c>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="14">
+        <v>45301</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3">
-        <v>45301</v>
-      </c>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <v>45301</v>
+      </c>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="14">
+        <v>45301</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3">
-        <v>45301</v>
-      </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="3">
+        <v>45301</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="14">
+        <v>45301</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="3">
-        <v>45301</v>
-      </c>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="3">
+        <v>45301</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="14">
+        <v>45301</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="3">
-        <v>45301</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="3">
+        <v>45301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1">
-        <v>2</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="14">
+        <v>45301</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3">
-        <v>45301</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="3">
+        <v>45301</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="14">
+        <v>45301</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>45301</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="E2:E6"/>
-    <mergeCell ref="E7:E8"/>
-  </mergeCells>
-  <conditionalFormatting sqref="E2:E6">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="1">
-      <formula>LEN(TRIM(E2))&gt;0</formula>
+  <conditionalFormatting sqref="F2:F6">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(F2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>